<commit_message>
Add 6 new compat card on openEuler 22.03LTS
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler22.03-LTS上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler22.03-LTS上两类平台板卡兼容清单.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Station\Gitee\website-v2\data\compatibility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76B3C4B-229B-4D88-9B37-24F0378BB42F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D67DA6F-C088-4A1D-9FE9-88E0A14CD3F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28130" windowHeight="12540" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
     <sheet name="板卡问题记录" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'openEuler22.03-LTS两类平台板卡兼容性'!$A$1:$U$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'openEuler22.03-LTS两类平台板卡兼容性'!$A$1:$U$42</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="252">
   <si>
     <t>vendorID</t>
   </si>
@@ -1038,6 +1038,142 @@
   </si>
   <si>
     <t>MT27808A0-FCCF-EV</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:12.8.0.4</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>ES3600C V5-3200GB</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>hns3</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>NIC</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>a221</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>14e4</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>15b3</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>16a1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>101b</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>1077</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>e3c1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>0029</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>bnx2x</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.03.30</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.03.31</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.04.01</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.04.02</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>47560B938AF29493141D36D0E2AE8D113A6174E9</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.6MB</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>195K</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.3MB</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.7MB</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qlogic</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mellanox</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>TM210</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>QLE3442-RJ-SP</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCX653105A-EFAT</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTL8211</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCM57840</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>CX6</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>03025VYQ</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>06310110</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>06030516</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -1276,7 +1412,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -1369,9 +1505,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1388,6 +1521,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1697,12 +1850,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O13" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.36328125" customWidth="1"/>
     <col min="6" max="6" width="19.7265625" customWidth="1"/>
     <col min="7" max="7" width="12.6328125" customWidth="1"/>
@@ -2158,7 +2312,7 @@
         <v>80</v>
       </c>
       <c r="P8" s="14"/>
-      <c r="Q8" s="54" t="s">
+      <c r="Q8" s="53" t="s">
         <v>215</v>
       </c>
       <c r="R8" s="14"/>
@@ -2268,7 +2422,7 @@
       <c r="P10" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="Q10" s="55" t="s">
+      <c r="Q10" s="54" t="s">
         <v>216</v>
       </c>
       <c r="R10" s="20"/>
@@ -2904,7 +3058,7 @@
       <c r="N22" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="O22" s="56" t="s">
+      <c r="O22" s="55" t="s">
         <v>217</v>
       </c>
       <c r="P22" s="26" t="s">
@@ -3195,8 +3349,8 @@
       <c r="G28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="14" t="s">
-        <v>23</v>
+      <c r="H28" s="56" t="s">
+        <v>218</v>
       </c>
       <c r="I28" s="14" t="s">
         <v>24</v>
@@ -3651,9 +3805,6 @@
       <c r="Q36" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="R36" s="26" t="s">
-        <v>200</v>
-      </c>
     </row>
     <row r="37" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
@@ -3707,9 +3858,6 @@
       <c r="Q37" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="R37" s="26" t="s">
-        <v>200</v>
-      </c>
     </row>
     <row r="38" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="35">
@@ -3721,7 +3869,7 @@
       <c r="C38" s="35">
         <v>8086</v>
       </c>
-      <c r="D38" s="53" t="s">
+      <c r="D38" s="52" t="s">
         <v>214</v>
       </c>
       <c r="E38" s="35" t="s">
@@ -3775,7 +3923,7 @@
       <c r="C39" s="35">
         <v>8086</v>
       </c>
-      <c r="D39" s="53" t="s">
+      <c r="D39" s="52" t="s">
         <v>214</v>
       </c>
       <c r="E39" s="26" t="s">
@@ -3922,65 +4070,267 @@
       </c>
     </row>
     <row r="42" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="35">
+      <c r="B42" s="42">
         <v>3714</v>
       </c>
-      <c r="C42" s="48" t="s">
+      <c r="C42" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="35">
+      <c r="D42" s="42">
         <v>5132</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="F42" s="35" t="s">
+      <c r="F42" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="35" t="s">
+      <c r="G42" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="H42" s="9" t="s">
+      <c r="H42" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="I42" s="35" t="s">
+      <c r="I42" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="J42" s="35" t="s">
+      <c r="J42" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="K42" s="35" t="s">
+      <c r="K42" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="L42" s="35" t="s">
+      <c r="L42" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="M42" s="35" t="s">
+      <c r="M42" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="N42" s="35" t="s">
+      <c r="N42" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="O42" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="P42" s="35" t="s">
+      <c r="O42" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="P42" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="35" t="s">
+      <c r="Q42" s="42" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:18" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="63" t="s">
+        <v>223</v>
+      </c>
+      <c r="C43" s="63" t="s">
+        <v>220</v>
+      </c>
+      <c r="D43" s="63" t="s">
+        <v>220</v>
+      </c>
+      <c r="E43" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="63" t="s">
+        <v>221</v>
+      </c>
+      <c r="H43" s="59"/>
+      <c r="I43" s="63" t="s">
+        <v>222</v>
+      </c>
+      <c r="J43" s="60" t="s">
+        <v>232</v>
+      </c>
+      <c r="K43" s="63" t="s">
+        <v>236</v>
+      </c>
+      <c r="L43" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="M43" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="N43" s="63" t="s">
+        <v>243</v>
+      </c>
+      <c r="O43" s="63" t="s">
+        <v>246</v>
+      </c>
+      <c r="P43" s="63" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q43" s="51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="63" t="s">
+        <v>224</v>
+      </c>
+      <c r="B44" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="C44" s="63" t="s">
+        <v>228</v>
+      </c>
+      <c r="D44" s="63" t="s">
+        <v>229</v>
+      </c>
+      <c r="E44" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="H44" s="59"/>
+      <c r="I44" s="63" t="s">
+        <v>222</v>
+      </c>
+      <c r="J44" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="K44" s="63" t="s">
+        <v>236</v>
+      </c>
+      <c r="L44" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="M44" s="63" t="s">
+        <v>241</v>
+      </c>
+      <c r="N44" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="O44" s="63" t="s">
+        <v>247</v>
+      </c>
+      <c r="P44" s="63" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q44" s="51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="B45" s="63" t="s">
+        <v>227</v>
+      </c>
+      <c r="C45" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="D45" s="63" t="s">
+        <v>230</v>
+      </c>
+      <c r="E45" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="H45" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="I45" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="J45" s="60" t="s">
+        <v>234</v>
+      </c>
+      <c r="K45" s="63" t="s">
+        <v>236</v>
+      </c>
+      <c r="L45" s="63" t="s">
+        <v>240</v>
+      </c>
+      <c r="M45" s="63" t="s">
+        <v>242</v>
+      </c>
+      <c r="N45" s="63" t="s">
+        <v>245</v>
+      </c>
+      <c r="O45" s="63" t="s">
+        <v>248</v>
+      </c>
+      <c r="P45" s="63" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q45" s="51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="63" t="s">
+        <v>224</v>
+      </c>
+      <c r="B46" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="C46" s="51">
+        <v>1077</v>
+      </c>
+      <c r="D46" s="63" t="s">
+        <v>229</v>
+      </c>
+      <c r="E46" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="H46" s="51"/>
+      <c r="I46" s="63" t="s">
+        <v>222</v>
+      </c>
+      <c r="J46" s="60" t="s">
+        <v>235</v>
+      </c>
+      <c r="K46" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="L46" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="M46" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="N46" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="O46" s="63" t="s">
+        <v>247</v>
+      </c>
+      <c r="P46" s="63" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q46" s="51" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" insertHyperlinks="0" autoFilter="0"/>
-  <autoFilter ref="A1:U37" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:U42" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10" xr:uid="{1496AB1C-C786-46AE-AD06-F8A883B01793}">
@@ -4001,10 +4351,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4016,43 +4366,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>180</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="51" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="50" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
-        <v>176</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A3" s="49" t="s">
         <v>204</v>
       </c>
-      <c r="B4" s="51" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4070,18 +4404,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <pixelatorList sheetStid="4"/>
-  <pixelatorList sheetStid="2"/>
-  <pixelatorList sheetStid="5"/>
-</pixelators>
+<comments xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<allowEditUser xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" hasInvisiblePropRange="0">
-  <rangeList sheetStid="4" master=""/>
-  <rangeList sheetStid="2" master=""/>
-</allowEditUser>
+<autofilters xmlns="https://web.wps.cn/et/2018/main">
+  <sheetItem sheetStid="4">
+    <filterData filterID="AK20210901:AK20210901JXNSXO4694343"/>
+    <autofilterInfo filterID="AK20210901:AK20210901JXNSXO4694343">
+      <autoFilter xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:U37"/>
+    </autofilterInfo>
+  </sheetItem>
+</autofilters>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4097,22 +4431,22 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<autofilters xmlns="https://web.wps.cn/et/2018/main">
-  <sheetItem sheetStid="4">
-    <filterData filterID="AK20210901:AK20210901JXNSXO4694343"/>
-    <autofilterInfo filterID="AK20210901:AK20210901JXNSXO4694343">
-      <autoFilter xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:U37"/>
-    </autofilterInfo>
-  </sheetItem>
-</autofilters>
+<allowEditUser xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" hasInvisiblePropRange="0">
+  <rangeList sheetStid="4" master=""/>
+  <rangeList sheetStid="2" master=""/>
+</allowEditUser>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <pixelatorList sheetStid="4"/>
+  <pixelatorList sheetStid="2"/>
+  <pixelatorList sheetStid="5"/>
+</pixelators>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06A0048C-2381-489B-AA07-9611017176EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
@@ -4121,7 +4455,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5607D9-04D2-4DE1-AC0E-A7772F01BC71}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5662047-3127-477A-AC3A-1D340467FB41}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
@@ -4139,7 +4473,7 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5662047-3127-477A-AC3A-1D340467FB41}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5607D9-04D2-4DE1-AC0E-A7772F01BC71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
@@ -4148,7 +4482,7 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06A0048C-2381-489B-AA07-9611017176EA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>

</xml_diff>

<commit_message>
add  broadcom nic card
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler22.03-LTS上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler22.03-LTS上两类平台板卡兼容清单.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Station\Gitee\website-v2\data\compatibility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwx1124290\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA590FEB-A2DA-4A1A-8693-A998BD8B0200}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openEuler22.03-LTS两类平台板卡兼容性" sheetId="1" r:id="rId1"/>
     <sheet name="板卡问题记录" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'openEuler22.03-LTS两类平台板卡兼容性'!$A$1:$U$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'openEuler22.03-LTS两类平台板卡兼容性'!$A$1:$U$46</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="245">
   <si>
     <t>vendorID</t>
   </si>
@@ -737,12 +736,87 @@
   <si>
     <t>https://repo.oepkgs.net/openEuler/rpm/openEuler-22.03-LTS/contrib/drivers/aarch64/Packages/cuda_11.6.1_510.47.03_linux_sbsa.run</t>
     <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>bnxt_en</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>16d7</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1402</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>406K</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.05.26</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>roadcom</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>06310148</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>CM57414</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCM957414A4142CC_08</t>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>207352D392184F5F7FBE52CE0A5C064DA1687B2</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -827,7 +901,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -935,6 +1009,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -946,7 +1055,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1053,11 +1162,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="常规 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="常规 2" xfId="2"/>
+    <cellStyle name="常规 3" xfId="3"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1437,30 +1566,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" customWidth="1"/>
-    <col min="6" max="6" width="19.7265625" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" customWidth="1"/>
-    <col min="8" max="8" width="14.36328125" customWidth="1"/>
-    <col min="10" max="10" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="19.75" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="14.375" customWidth="1"/>
+    <col min="10" max="10" width="12.625" customWidth="1"/>
     <col min="11" max="11" width="41" customWidth="1"/>
-    <col min="12" max="12" width="9.6328125" customWidth="1"/>
-    <col min="13" max="13" width="9.81640625" customWidth="1"/>
-    <col min="14" max="14" width="14.7265625" customWidth="1"/>
-    <col min="15" max="15" width="28.08984375" customWidth="1"/>
+    <col min="12" max="12" width="9.625" customWidth="1"/>
+    <col min="13" max="13" width="9.875" customWidth="1"/>
+    <col min="14" max="14" width="20.625" customWidth="1"/>
+    <col min="15" max="15" width="28.125" customWidth="1"/>
     <col min="17" max="17" width="138" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="7" customFormat="1" ht="28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1519,7 +1648,7 @@
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
@@ -1576,7 +1705,7 @@
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
@@ -1633,7 +1762,7 @@
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
     </row>
-    <row r="4" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>37</v>
       </c>
@@ -1688,9 +1817,9 @@
       <c r="R4" s="9"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-    </row>
-    <row r="5" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U4" s="58"/>
+    </row>
+    <row r="5" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
@@ -1745,9 +1874,9 @@
       <c r="R5" s="9"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-    </row>
-    <row r="6" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="7"/>
+    </row>
+    <row r="6" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
         <v>60</v>
       </c>
@@ -1800,9 +1929,9 @@
       <c r="R6" s="9"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-    </row>
-    <row r="7" spans="1:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="U6" s="7"/>
+    </row>
+    <row r="7" spans="1:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>48</v>
       </c>
@@ -1857,9 +1986,9 @@
       <c r="R7" s="9"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-    </row>
-    <row r="8" spans="1:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="U7" s="59"/>
+    </row>
+    <row r="8" spans="1:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>79</v>
       </c>
@@ -1910,9 +2039,9 @@
       <c r="R8" s="9"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-    </row>
-    <row r="9" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="58"/>
+    </row>
+    <row r="9" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>60</v>
       </c>
@@ -1965,9 +2094,9 @@
       <c r="R9" s="9"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-    </row>
-    <row r="10" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>79</v>
       </c>
@@ -2020,9 +2149,9 @@
       <c r="R10" s="17"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-    </row>
-    <row r="11" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U10" s="59"/>
+    </row>
+    <row r="11" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>99</v>
       </c>
@@ -2075,8 +2204,9 @@
         <v>32</v>
       </c>
       <c r="R11" s="9"/>
-    </row>
-    <row r="12" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="51"/>
+    </row>
+    <row r="12" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="21" t="s">
         <v>112</v>
       </c>
@@ -2130,7 +2260,7 @@
       </c>
       <c r="R12" s="9"/>
     </row>
-    <row r="13" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="21" t="s">
         <v>112</v>
       </c>
@@ -2183,7 +2313,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="21" t="s">
         <v>99</v>
       </c>
@@ -2235,8 +2365,9 @@
       <c r="Q14" s="23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U14" s="56"/>
+    </row>
+    <row r="15" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="21" t="s">
         <v>99</v>
       </c>
@@ -2288,8 +2419,9 @@
       <c r="Q15" s="23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="51"/>
+    </row>
+    <row r="16" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="21" t="s">
         <v>112</v>
       </c>
@@ -2342,7 +2474,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="21" t="s">
         <v>112</v>
       </c>
@@ -2395,7 +2527,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="21" t="s">
         <v>99</v>
       </c>
@@ -2447,8 +2579,9 @@
       <c r="Q18" s="23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U18" s="56"/>
+    </row>
+    <row r="19" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="21" t="s">
         <v>99</v>
       </c>
@@ -2501,7 +2634,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="21" t="s">
         <v>99</v>
       </c>
@@ -2554,7 +2687,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
         <v>112</v>
       </c>
@@ -2606,8 +2739,9 @@
       <c r="Q21" s="23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U21" s="51"/>
+    </row>
+    <row r="22" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
         <v>60</v>
       </c>
@@ -2657,7 +2791,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
         <v>60</v>
       </c>
@@ -2707,7 +2841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
         <v>37</v>
       </c>
@@ -2759,8 +2893,9 @@
       <c r="Q24" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U24" s="56"/>
+    </row>
+    <row r="25" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
         <v>18</v>
       </c>
@@ -2813,7 +2948,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
         <v>18</v>
       </c>
@@ -2866,7 +3001,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
         <v>18</v>
       </c>
@@ -2919,7 +3054,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>18</v>
       </c>
@@ -2972,7 +3107,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
         <v>18</v>
       </c>
@@ -3025,7 +3160,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
         <v>18</v>
       </c>
@@ -3082,7 +3217,7 @@
       <c r="T30" s="20"/>
       <c r="U30" s="20"/>
     </row>
-    <row r="31" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
         <v>99</v>
       </c>
@@ -3131,11 +3266,11 @@
       <c r="P31" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="Q31" s="19" t="s">
+      <c r="Q31" s="50" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
         <v>48</v>
       </c>
@@ -3184,11 +3319,15 @@
       <c r="P32" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="Q32" s="17" t="s">
+      <c r="Q32" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
+    </row>
+    <row r="33" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="s">
         <v>79</v>
       </c>
@@ -3235,11 +3374,11 @@
       <c r="P33" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="Q33" s="48" t="s">
+      <c r="Q33" s="52" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A34" s="20" t="s">
         <v>112</v>
       </c>
@@ -3288,11 +3427,15 @@
       <c r="P34" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="Q34" s="23" t="s">
+      <c r="Q34" s="25" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R34" s="51"/>
+      <c r="S34" s="51"/>
+      <c r="T34" s="51"/>
+      <c r="U34" s="51"/>
+    </row>
+    <row r="35" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A35" s="29" t="s">
         <v>112</v>
       </c>
@@ -3341,11 +3484,11 @@
       <c r="P35" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="Q35" s="23" t="s">
+      <c r="Q35" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="31" t="s">
         <v>112</v>
       </c>
@@ -3394,11 +3537,11 @@
       <c r="P36" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="Q36" s="25" t="s">
+      <c r="Q36" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A37" s="34">
         <v>8086</v>
       </c>
@@ -3451,8 +3594,11 @@
       <c r="R37" s="20" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+    </row>
+    <row r="38" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A38" s="34">
         <v>8086</v>
       </c>
@@ -3505,8 +3651,11 @@
       <c r="R38" s="20" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+    </row>
+    <row r="39" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="26" t="s">
         <v>79</v>
       </c>
@@ -3553,11 +3702,11 @@
       <c r="P39" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="Q39" s="49" t="s">
+      <c r="Q39" s="53" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
         <v>79</v>
       </c>
@@ -3608,7 +3757,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="41" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A41" s="33" t="s">
         <v>48</v>
       </c>
@@ -3661,7 +3810,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" s="41" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A42" s="38" t="s">
         <v>48</v>
       </c>
@@ -3711,8 +3860,12 @@
       <c r="Q42" s="26" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R42" s="57"/>
+      <c r="S42" s="57"/>
+      <c r="T42" s="57"/>
+      <c r="U42" s="57"/>
+    </row>
+    <row r="43" spans="1:21" s="41" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A43" s="39" t="s">
         <v>212</v>
       </c>
@@ -3762,8 +3915,12 @@
       <c r="Q43" s="26" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R43" s="57"/>
+      <c r="S43" s="57"/>
+      <c r="T43" s="57"/>
+      <c r="U43" s="57"/>
+    </row>
+    <row r="44" spans="1:21" s="41" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="39" t="s">
         <v>112</v>
       </c>
@@ -3812,11 +3969,11 @@
       <c r="P44" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="Q44" s="26" t="s">
+      <c r="Q44" s="54" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A45" s="39" t="s">
         <v>212</v>
       </c>
@@ -3866,22 +4023,81 @@
       <c r="Q45" s="26" t="s">
         <v>32</v>
       </c>
+      <c r="R45" s="20"/>
+      <c r="S45" s="20"/>
+      <c r="T45" s="20"/>
+      <c r="U45" s="20"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A46" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="B46" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="H46" s="26"/>
+      <c r="I46" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="J46" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="K46" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="L46" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="M46" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="N46" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="O46" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="P46" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q46" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="R46" s="56"/>
+      <c r="S46" s="56"/>
+      <c r="T46" s="56"/>
+      <c r="U46" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U41" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:U46"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
       <formula1>"aarch64,x86_64"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="Q10" r:id="rId1" xr:uid="{56C7505E-31E3-44A8-8711-B2DBD6BA8BE4}"/>
-    <hyperlink ref="Q8" r:id="rId2" xr:uid="{849B5B12-9AD1-4285-9018-34CBC3A2E6CD}"/>
-    <hyperlink ref="Q33" r:id="rId3" xr:uid="{A452A69E-32A6-4A99-B45C-835DF8A6B211}"/>
-    <hyperlink ref="Q39" r:id="rId4" xr:uid="{346646CB-0781-4F18-BCB9-A8D42D045FF3}"/>
-    <hyperlink ref="Q40" r:id="rId5" xr:uid="{A4A30801-2F7D-40F5-A5F3-1196628CF4C0}"/>
+    <hyperlink ref="Q10" r:id="rId1"/>
+    <hyperlink ref="Q8" r:id="rId2"/>
+    <hyperlink ref="Q33" r:id="rId3"/>
+    <hyperlink ref="Q39" r:id="rId4"/>
+    <hyperlink ref="Q40" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -3889,22 +4105,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" style="43" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="43" customWidth="1"/>
+    <col min="1" max="1" width="15.75" style="43" customWidth="1"/>
+    <col min="2" max="2" width="21.125" style="43" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="43" customWidth="1"/>
     <col min="4" max="1024" width="9" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="44" t="s">
         <v>229</v>
       </c>
@@ -3913,7 +4129,7 @@
       </c>
       <c r="C1" s="45"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="26" t="s">
         <v>198</v>
       </c>
@@ -3921,7 +4137,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="20" t="s">
         <v>198</v>
       </c>

</xml_diff>

<commit_message>
update sp350 sp351 chipModel
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler22.03-LTS上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler22.03-LTS上两类平台板卡兼容清单.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="295">
   <si>
     <t>vendorID</t>
   </si>
@@ -494,7 +494,7 @@
     <t>SP351</t>
   </si>
   <si>
-    <t>MT27808A0-FCCF-EV</t>
+    <t>CX5</t>
   </si>
   <si>
     <t>03024QAY</t>
@@ -600,9 +600,6 @@
   </si>
   <si>
     <t>MCX516A-CCAT</t>
-  </si>
-  <si>
-    <t>CX5</t>
   </si>
   <si>
     <t>06310158</t>
@@ -964,9 +961,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
@@ -1025,8 +1022,29 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -1034,7 +1052,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1048,29 +1074,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1086,6 +1097,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -1093,29 +1120,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1131,38 +1159,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1189,7 +1186,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1201,7 +1288,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1213,31 +1330,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1249,55 +1354,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1309,67 +1366,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1545,33 +1542,22 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1592,16 +1578,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1609,155 +1604,157 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
@@ -1847,7 +1844,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1855,6 +1851,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2315,8 +2312,8 @@
   <sheetPr/>
   <dimension ref="A1:AB81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3477,7 +3474,7 @@
       <c r="N21" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="O21" s="35" t="s">
+      <c r="O21" s="20" t="s">
         <v>158</v>
       </c>
       <c r="P21" s="5" t="s">
@@ -4115,10 +4112,10 @@
       <c r="N33" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="O33" s="36" t="s">
+      <c r="O33" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="P33" s="37" t="s">
+      <c r="P33" s="36" t="s">
         <v>191</v>
       </c>
       <c r="Q33" s="59" t="s">
@@ -4168,7 +4165,7 @@
       <c r="N34" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="O34" s="5" t="s">
+      <c r="O34" s="20" t="s">
         <v>158</v>
       </c>
       <c r="P34" s="5" t="s">
@@ -4226,10 +4223,10 @@
         <v>193</v>
       </c>
       <c r="O35" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="P35" s="20" t="s">
         <v>194</v>
-      </c>
-      <c r="P35" s="20" t="s">
-        <v>195</v>
       </c>
       <c r="Q35" s="12" t="s">
         <v>32</v>
@@ -4279,10 +4276,10 @@
         <v>193</v>
       </c>
       <c r="O36" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="P36" s="22" t="s">
         <v>194</v>
-      </c>
-      <c r="P36" s="22" t="s">
-        <v>195</v>
       </c>
       <c r="Q36" s="12" t="s">
         <v>32</v>
@@ -4299,7 +4296,7 @@
         <v>8086</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E37" s="24" t="s">
         <v>21</v>
@@ -4308,38 +4305,38 @@
         <v>22</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H37" s="24"/>
       <c r="I37" s="24" t="s">
         <v>53</v>
       </c>
       <c r="J37" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K37" s="24" t="s">
         <v>182</v>
       </c>
       <c r="L37" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M37" s="24" t="s">
         <v>66</v>
       </c>
       <c r="N37" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O37" s="24" t="s">
         <v>66</v>
       </c>
       <c r="P37" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q37" s="26" t="s">
         <v>32</v>
       </c>
       <c r="R37" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
@@ -4356,7 +4353,7 @@
         <v>8086</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E38" s="26" t="s">
         <v>82</v>
@@ -4365,38 +4362,38 @@
         <v>22</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26" t="s">
         <v>53</v>
       </c>
       <c r="J38" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K38" s="26" t="s">
         <v>91</v>
       </c>
       <c r="L38" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M38" s="26" t="s">
         <v>66</v>
       </c>
       <c r="N38" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O38" s="26" t="s">
         <v>66</v>
       </c>
       <c r="P38" s="26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q38" s="26" t="s">
         <v>32</v>
       </c>
       <c r="R38" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
@@ -4431,7 +4428,7 @@
         <v>85</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4" t="s">
@@ -4450,7 +4447,7 @@
         <v>99</v>
       </c>
       <c r="Q39" s="60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -4482,7 +4479,7 @@
         <v>85</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4" t="s">
@@ -4501,7 +4498,7 @@
         <v>191</v>
       </c>
       <c r="Q40" s="61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -4533,13 +4530,13 @@
         <v>74</v>
       </c>
       <c r="J41" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K41" s="22" t="s">
         <v>91</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M41" s="22" t="s">
         <v>56</v>
@@ -4562,13 +4559,13 @@
         <v>48</v>
       </c>
       <c r="B42" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="C42" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="C42" s="27" t="s">
-        <v>208</v>
-      </c>
       <c r="D42" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>21</v>
@@ -4577,32 +4574,32 @@
         <v>22</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H42" s="27"/>
       <c r="I42" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J42" s="38" t="s">
-        <v>210</v>
+      <c r="J42" s="37" t="s">
+        <v>209</v>
       </c>
       <c r="K42" s="27" t="s">
         <v>182</v>
       </c>
       <c r="L42" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>56</v>
       </c>
       <c r="N42" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="O42" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="O42" s="27" t="s">
+      <c r="P42" s="27" t="s">
         <v>213</v>
-      </c>
-      <c r="P42" s="27" t="s">
-        <v>214</v>
       </c>
       <c r="Q42" s="4" t="s">
         <v>32</v>
@@ -4614,16 +4611,16 @@
     </row>
     <row r="43" s="7" customFormat="1" spans="1:21">
       <c r="A43" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B43" s="27" t="s">
         <v>215</v>
-      </c>
-      <c r="B43" s="27" t="s">
-        <v>216</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>21</v>
@@ -4632,32 +4629,32 @@
         <v>22</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H43" s="27"/>
       <c r="I43" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J43" s="38" t="s">
-        <v>219</v>
+      <c r="J43" s="37" t="s">
+        <v>218</v>
       </c>
       <c r="K43" s="27" t="s">
         <v>182</v>
       </c>
       <c r="L43" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M43" s="27" t="s">
         <v>44</v>
       </c>
       <c r="N43" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="O43" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="O43" s="27" t="s">
+      <c r="P43" s="27" t="s">
         <v>222</v>
-      </c>
-      <c r="P43" s="27" t="s">
-        <v>223</v>
       </c>
       <c r="Q43" s="4" t="s">
         <v>32</v>
@@ -4672,13 +4669,13 @@
         <v>114</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>114</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>21</v>
@@ -4695,8 +4692,8 @@
       <c r="I44" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="J44" s="38" t="s">
-        <v>226</v>
+      <c r="J44" s="37" t="s">
+        <v>225</v>
       </c>
       <c r="K44" s="27" t="s">
         <v>182</v>
@@ -4708,13 +4705,13 @@
         <v>120</v>
       </c>
       <c r="N44" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="O44" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="O44" s="27" t="s">
+      <c r="P44" s="27" t="s">
         <v>228</v>
-      </c>
-      <c r="P44" s="27" t="s">
-        <v>229</v>
       </c>
       <c r="Q44" s="63" t="s">
         <v>32</v>
@@ -4722,16 +4719,16 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B45" s="27" t="s">
         <v>215</v>
-      </c>
-      <c r="B45" s="27" t="s">
-        <v>216</v>
       </c>
       <c r="C45" s="4">
         <v>1077</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>82</v>
@@ -4740,32 +4737,32 @@
         <v>22</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J45" s="38" t="s">
-        <v>230</v>
+      <c r="J45" s="37" t="s">
+        <v>229</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="L45" s="38" t="s">
-        <v>231</v>
-      </c>
-      <c r="M45" s="38" t="s">
+      <c r="L45" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="M45" s="37" t="s">
         <v>44</v>
       </c>
       <c r="N45" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="O45" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="O45" s="27" t="s">
+      <c r="P45" s="27" t="s">
         <v>222</v>
-      </c>
-      <c r="P45" s="27" t="s">
-        <v>223</v>
       </c>
       <c r="Q45" s="4" t="s">
         <v>32</v>
@@ -4777,16 +4774,16 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B46" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="D46" s="27" t="s">
         <v>232</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>233</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>21</v>
@@ -4795,32 +4792,32 @@
         <v>22</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J46" s="38" t="s">
+      <c r="J46" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="K46" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="K46" s="35" t="s">
+      <c r="L46" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="L46" s="27" t="s">
+      <c r="M46" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="M46" s="35" t="s">
+      <c r="N46" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="N46" s="35" t="s">
+      <c r="O46" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="O46" s="35" t="s">
+      <c r="P46" s="27" t="s">
         <v>240</v>
-      </c>
-      <c r="P46" s="27" t="s">
-        <v>241</v>
       </c>
       <c r="Q46" s="64" t="s">
         <v>32</v>
@@ -4832,16 +4829,16 @@
     </row>
     <row r="47" ht="27" spans="1:28">
       <c r="A47" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="B47" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="C47" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="D47" s="30" t="s">
         <v>243</v>
-      </c>
-      <c r="C47" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="D47" s="30" t="s">
-        <v>244</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>82</v>
@@ -4850,35 +4847,35 @@
         <v>22</v>
       </c>
       <c r="G47" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H47" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H47" s="30" t="s">
+      <c r="I47" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I47" s="30" t="s">
+      <c r="J47" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="K47" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J47" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="K47" s="39" t="s">
+      <c r="L47" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L47" s="30" t="s">
+      <c r="M47" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="M47" s="30" t="s">
+      <c r="N47" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="N47" s="30" t="s">
+      <c r="O47" s="30" t="s">
         <v>251</v>
-      </c>
-      <c r="O47" s="30" t="s">
-        <v>252</v>
       </c>
       <c r="P47" s="40"/>
       <c r="Q47" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R47" s="62"/>
       <c r="S47" s="62"/>
@@ -4894,16 +4891,16 @@
     </row>
     <row r="48" ht="27" spans="1:28">
       <c r="A48" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="B48" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="C48" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="D48" s="30" t="s">
         <v>243</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>244</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>82</v>
@@ -4912,35 +4909,35 @@
         <v>22</v>
       </c>
       <c r="G48" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H48" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H48" s="30" t="s">
+      <c r="I48" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I48" s="30" t="s">
+      <c r="J48" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="K48" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J48" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="K48" s="39" t="s">
+      <c r="L48" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L48" s="30" t="s">
+      <c r="M48" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="M48" s="30" t="s">
-        <v>250</v>
-      </c>
       <c r="N48" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="O48" s="30" t="s">
         <v>254</v>
-      </c>
-      <c r="O48" s="30" t="s">
-        <v>255</v>
       </c>
       <c r="P48" s="41"/>
       <c r="Q48" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R48" s="62"/>
       <c r="S48" s="62"/>
@@ -4956,16 +4953,16 @@
     </row>
     <row r="49" ht="27" spans="1:28">
       <c r="A49" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="B49" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="B49" s="29" t="s">
-        <v>257</v>
-      </c>
       <c r="C49" s="28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>82</v>
@@ -4974,35 +4971,35 @@
         <v>22</v>
       </c>
       <c r="G49" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H49" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H49" s="30" t="s">
+      <c r="I49" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I49" s="30" t="s">
+      <c r="J49" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="K49" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J49" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="K49" s="39" t="s">
+      <c r="L49" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L49" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M49" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="N49" s="30" t="s">
         <v>258</v>
       </c>
-      <c r="N49" s="30" t="s">
+      <c r="O49" s="30" t="s">
         <v>259</v>
-      </c>
-      <c r="O49" s="30" t="s">
-        <v>260</v>
       </c>
       <c r="P49" s="42"/>
       <c r="Q49" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R49" s="62"/>
       <c r="S49" s="62"/>
@@ -5018,16 +5015,16 @@
     </row>
     <row r="50" ht="27" spans="1:28">
       <c r="A50" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="B50" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="B50" s="29" t="s">
-        <v>257</v>
-      </c>
       <c r="C50" s="28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>82</v>
@@ -5036,35 +5033,35 @@
         <v>22</v>
       </c>
       <c r="G50" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H50" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H50" s="30" t="s">
+      <c r="I50" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I50" s="30" t="s">
+      <c r="J50" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="K50" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J50" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="K50" s="39" t="s">
+      <c r="L50" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L50" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M50" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N50" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O50" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P50" s="43"/>
       <c r="Q50" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R50" s="62"/>
       <c r="S50" s="62"/>
@@ -5080,16 +5077,16 @@
     </row>
     <row r="51" ht="27" spans="1:28">
       <c r="A51" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B51" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B51" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C51" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>82</v>
@@ -5098,35 +5095,35 @@
         <v>22</v>
       </c>
       <c r="G51" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H51" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H51" s="30" t="s">
+      <c r="I51" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I51" s="30" t="s">
+      <c r="J51" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="K51" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J51" s="28" t="s">
+      <c r="L51" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="M51" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="K51" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="L51" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="M51" s="30" t="s">
+      <c r="N51" s="30" t="s">
         <v>265</v>
       </c>
-      <c r="N51" s="30" t="s">
+      <c r="O51" s="44" t="s">
         <v>266</v>
-      </c>
-      <c r="O51" s="44" t="s">
-        <v>267</v>
       </c>
       <c r="P51" s="45"/>
       <c r="Q51" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R51" s="62"/>
       <c r="S51" s="62"/>
@@ -5142,16 +5139,16 @@
     </row>
     <row r="52" ht="27" spans="1:28">
       <c r="A52" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B52" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B52" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C52" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>82</v>
@@ -5160,35 +5157,35 @@
         <v>22</v>
       </c>
       <c r="G52" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H52" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H52" s="30" t="s">
+      <c r="I52" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I52" s="30" t="s">
+      <c r="J52" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="K52" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J52" s="28" t="s">
+      <c r="L52" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="M52" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="K52" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="L52" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="M52" s="30" t="s">
-        <v>265</v>
-      </c>
       <c r="N52" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O52" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P52" s="43"/>
       <c r="Q52" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R52" s="62"/>
       <c r="S52" s="62"/>
@@ -5204,16 +5201,16 @@
     </row>
     <row r="53" ht="27" spans="1:28">
       <c r="A53" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C53" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>82</v>
@@ -5222,35 +5219,35 @@
         <v>22</v>
       </c>
       <c r="G53" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H53" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="I53" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I53" s="30" t="s">
+      <c r="J53" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="K53" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J53" s="28" t="s">
+      <c r="L53" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="M53" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="N53" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="K53" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="L53" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="M53" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="N53" s="30" t="s">
-        <v>271</v>
-      </c>
       <c r="O53" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P53" s="30"/>
       <c r="Q53" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R53" s="62"/>
       <c r="S53" s="62"/>
@@ -5266,16 +5263,16 @@
     </row>
     <row r="54" spans="1:28">
       <c r="A54" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="B54" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="B54" s="31" t="s">
-        <v>273</v>
-      </c>
       <c r="C54" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>82</v>
@@ -5286,21 +5283,21 @@
       <c r="G54" s="30"/>
       <c r="H54" s="30"/>
       <c r="I54" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J54" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K54" s="39"/>
       <c r="L54" s="30"/>
       <c r="M54" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="N54" s="46" t="s">
         <v>274</v>
       </c>
-      <c r="N54" s="46" t="s">
+      <c r="O54" s="44" t="s">
         <v>275</v>
-      </c>
-      <c r="O54" s="44" t="s">
-        <v>276</v>
       </c>
       <c r="P54" s="31"/>
       <c r="Q54" s="65"/>
@@ -5318,16 +5315,16 @@
     </row>
     <row r="55" spans="1:28">
       <c r="A55" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="B55" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="B55" s="31" t="s">
-        <v>273</v>
-      </c>
       <c r="C55" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>82</v>
@@ -5338,21 +5335,21 @@
       <c r="G55" s="30"/>
       <c r="H55" s="30"/>
       <c r="I55" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J55" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K55" s="39"/>
       <c r="L55" s="30"/>
       <c r="M55" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N55" s="47" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O55" s="44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P55" s="47"/>
       <c r="Q55" s="65"/>
@@ -5370,16 +5367,16 @@
     </row>
     <row r="56" spans="1:28">
       <c r="A56" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="B56" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="B56" s="31" t="s">
-        <v>273</v>
-      </c>
       <c r="C56" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>82</v>
@@ -5390,21 +5387,21 @@
       <c r="G56" s="30"/>
       <c r="H56" s="30"/>
       <c r="I56" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J56" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K56" s="39"/>
       <c r="L56" s="30"/>
       <c r="M56" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N56" s="28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O56" s="44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P56" s="48"/>
       <c r="Q56" s="65"/>
@@ -5422,16 +5419,16 @@
     </row>
     <row r="57" ht="27" spans="1:28">
       <c r="A57" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B57" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B57" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C57" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>82</v>
@@ -5440,35 +5437,35 @@
         <v>22</v>
       </c>
       <c r="G57" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H57" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H57" s="30" t="s">
+      <c r="I57" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I57" s="30" t="s">
+      <c r="J57" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="K57" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J57" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="K57" s="39" t="s">
+      <c r="L57" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L57" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M57" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N57" s="28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O57" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P57" s="48"/>
       <c r="Q57" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R57" s="62"/>
       <c r="S57" s="62"/>
@@ -5484,16 +5481,16 @@
     </row>
     <row r="58" ht="27" spans="1:28">
       <c r="A58" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B58" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B58" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C58" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>82</v>
@@ -5502,35 +5499,35 @@
         <v>22</v>
       </c>
       <c r="G58" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H58" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H58" s="30" t="s">
+      <c r="I58" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I58" s="30" t="s">
+      <c r="J58" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="K58" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J58" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="K58" s="39" t="s">
+      <c r="L58" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L58" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M58" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="N58" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="N58" s="28" t="s">
+      <c r="O58" s="44" t="s">
         <v>281</v>
-      </c>
-      <c r="O58" s="44" t="s">
-        <v>282</v>
       </c>
       <c r="P58" s="29"/>
       <c r="Q58" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R58" s="66"/>
       <c r="S58" s="66"/>
@@ -5546,16 +5543,16 @@
     </row>
     <row r="59" ht="27" spans="1:28">
       <c r="A59" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B59" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B59" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C59" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>82</v>
@@ -5564,35 +5561,35 @@
         <v>22</v>
       </c>
       <c r="G59" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H59" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H59" s="30" t="s">
+      <c r="I59" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I59" s="30" t="s">
+      <c r="J59" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="K59" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J59" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="K59" s="39" t="s">
+      <c r="L59" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L59" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M59" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N59" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O59" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P59" s="29"/>
       <c r="Q59" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R59" s="66"/>
       <c r="S59" s="66"/>
@@ -5608,16 +5605,16 @@
     </row>
     <row r="60" ht="27" spans="1:28">
       <c r="A60" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B60" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B60" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C60" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D60" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>82</v>
@@ -5626,35 +5623,35 @@
         <v>22</v>
       </c>
       <c r="G60" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H60" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H60" s="30" t="s">
+      <c r="I60" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I60" s="30" t="s">
+      <c r="J60" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="K60" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J60" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="K60" s="39" t="s">
+      <c r="L60" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L60" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M60" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N60" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O60" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P60" s="29"/>
       <c r="Q60" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R60" s="66"/>
       <c r="S60" s="66"/>
@@ -5670,16 +5667,16 @@
     </row>
     <row r="61" ht="27" spans="1:28">
       <c r="A61" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B61" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B61" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C61" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>82</v>
@@ -5688,35 +5685,35 @@
         <v>22</v>
       </c>
       <c r="G61" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H61" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H61" s="30" t="s">
+      <c r="I61" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I61" s="30" t="s">
+      <c r="J61" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="K61" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J61" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="K61" s="39" t="s">
+      <c r="L61" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L61" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M61" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N61" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O61" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P61" s="31"/>
       <c r="Q61" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R61" s="62"/>
       <c r="S61" s="62"/>
@@ -5732,16 +5729,16 @@
     </row>
     <row r="62" ht="27" spans="1:28">
       <c r="A62" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B62" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B62" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C62" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>82</v>
@@ -5750,35 +5747,35 @@
         <v>22</v>
       </c>
       <c r="G62" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H62" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H62" s="30" t="s">
+      <c r="I62" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I62" s="30" t="s">
+      <c r="J62" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="K62" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J62" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="K62" s="39" t="s">
+      <c r="L62" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L62" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M62" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N62" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O62" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P62" s="31"/>
       <c r="Q62" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R62" s="62"/>
       <c r="S62" s="62"/>
@@ -5794,16 +5791,16 @@
     </row>
     <row r="63" ht="27" spans="1:28">
       <c r="A63" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B63" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B63" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C63" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>82</v>
@@ -5812,35 +5809,35 @@
         <v>22</v>
       </c>
       <c r="G63" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H63" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H63" s="30" t="s">
+      <c r="I63" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I63" s="30" t="s">
+      <c r="J63" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="K63" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J63" s="28" t="s">
+      <c r="L63" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="M63" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="K63" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="L63" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="M63" s="30" t="s">
-        <v>265</v>
-      </c>
       <c r="N63" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O63" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P63" s="49"/>
       <c r="Q63" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R63" s="62"/>
       <c r="S63" s="62"/>
@@ -5856,16 +5853,16 @@
     </row>
     <row r="64" ht="27" spans="1:28">
       <c r="A64" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B64" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B64" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C64" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>82</v>
@@ -5874,35 +5871,35 @@
         <v>22</v>
       </c>
       <c r="G64" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H64" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H64" s="30" t="s">
+      <c r="I64" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I64" s="30" t="s">
+      <c r="J64" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="K64" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J64" s="28" t="s">
+      <c r="L64" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="M64" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="K64" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="L64" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="M64" s="30" t="s">
-        <v>265</v>
-      </c>
       <c r="N64" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O64" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P64" s="43"/>
       <c r="Q64" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R64" s="62"/>
       <c r="S64" s="62"/>
@@ -5918,16 +5915,16 @@
     </row>
     <row r="65" ht="27" spans="1:28">
       <c r="A65" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B65" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B65" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C65" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>82</v>
@@ -5936,35 +5933,35 @@
         <v>22</v>
       </c>
       <c r="G65" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H65" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H65" s="30" t="s">
+      <c r="I65" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I65" s="30" t="s">
+      <c r="J65" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="K65" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J65" s="28" t="s">
+      <c r="L65" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="M65" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="K65" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="L65" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="M65" s="30" t="s">
-        <v>265</v>
-      </c>
       <c r="N65" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O65" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P65" s="43"/>
       <c r="Q65" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R65" s="62"/>
       <c r="S65" s="62"/>
@@ -5980,16 +5977,16 @@
     </row>
     <row r="66" ht="27" spans="1:28">
       <c r="A66" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B66" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B66" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C66" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>82</v>
@@ -5998,35 +5995,35 @@
         <v>22</v>
       </c>
       <c r="G66" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H66" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H66" s="30" t="s">
+      <c r="I66" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I66" s="30" t="s">
+      <c r="J66" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="K66" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J66" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="K66" s="39" t="s">
+      <c r="L66" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L66" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M66" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N66" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O66" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P66" s="47"/>
       <c r="Q66" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R66" s="62"/>
       <c r="S66" s="62"/>
@@ -6042,16 +6039,16 @@
     </row>
     <row r="67" ht="27" spans="1:28">
       <c r="A67" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B67" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B67" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C67" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>82</v>
@@ -6060,35 +6057,35 @@
         <v>22</v>
       </c>
       <c r="G67" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H67" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H67" s="30" t="s">
+      <c r="I67" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I67" s="30" t="s">
+      <c r="J67" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="K67" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J67" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="K67" s="39" t="s">
+      <c r="L67" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L67" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M67" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N67" s="28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O67" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P67" s="48"/>
       <c r="Q67" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R67" s="62"/>
       <c r="S67" s="62"/>
@@ -6104,16 +6101,16 @@
     </row>
     <row r="68" ht="27" spans="1:28">
       <c r="A68" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B68" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B68" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C68" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D68" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E68" s="67" t="s">
         <v>21</v>
@@ -6122,35 +6119,35 @@
         <v>22</v>
       </c>
       <c r="G68" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H68" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H68" s="30" t="s">
+      <c r="I68" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I68" s="30" t="s">
+      <c r="J68" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K68" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J68" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K68" s="39" t="s">
+      <c r="L68" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L68" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M68" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="N68" s="30" t="s">
         <v>265</v>
       </c>
-      <c r="N68" s="30" t="s">
+      <c r="O68" s="44" t="s">
         <v>266</v>
-      </c>
-      <c r="O68" s="44" t="s">
-        <v>267</v>
       </c>
       <c r="P68" s="45"/>
       <c r="Q68" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R68" s="62"/>
       <c r="S68" s="62"/>
@@ -6166,16 +6163,16 @@
     </row>
     <row r="69" ht="27" spans="1:28">
       <c r="A69" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B69" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B69" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C69" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E69" s="67" t="s">
         <v>21</v>
@@ -6184,35 +6181,35 @@
         <v>22</v>
       </c>
       <c r="G69" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H69" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H69" s="30" t="s">
+      <c r="I69" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I69" s="30" t="s">
+      <c r="J69" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K69" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J69" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K69" s="39" t="s">
+      <c r="L69" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L69" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M69" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N69" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O69" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P69" s="43"/>
       <c r="Q69" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R69" s="62"/>
       <c r="S69" s="62"/>
@@ -6228,16 +6225,16 @@
     </row>
     <row r="70" ht="27" spans="1:28">
       <c r="A70" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E70" s="67" t="s">
         <v>21</v>
@@ -6246,35 +6243,35 @@
         <v>22</v>
       </c>
       <c r="G70" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H70" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H70" s="30" t="s">
+      <c r="I70" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I70" s="30" t="s">
+      <c r="J70" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K70" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J70" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K70" s="39" t="s">
+      <c r="L70" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L70" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M70" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N70" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O70" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P70" s="30"/>
       <c r="Q70" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R70" s="62"/>
       <c r="S70" s="62"/>
@@ -6290,16 +6287,16 @@
     </row>
     <row r="71" ht="27" spans="1:28">
       <c r="A71" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B71" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B71" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C71" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E71" s="67" t="s">
         <v>21</v>
@@ -6308,35 +6305,35 @@
         <v>22</v>
       </c>
       <c r="G71" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H71" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H71" s="30" t="s">
+      <c r="I71" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I71" s="30" t="s">
+      <c r="J71" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K71" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J71" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K71" s="39" t="s">
+      <c r="L71" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L71" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M71" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N71" s="28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O71" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P71" s="48"/>
       <c r="Q71" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R71" s="62"/>
       <c r="S71" s="62"/>
@@ -6352,16 +6349,16 @@
     </row>
     <row r="72" ht="27" spans="1:28">
       <c r="A72" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B72" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B72" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C72" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E72" s="67" t="s">
         <v>21</v>
@@ -6370,35 +6367,35 @@
         <v>22</v>
       </c>
       <c r="G72" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H72" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H72" s="30" t="s">
+      <c r="I72" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I72" s="30" t="s">
+      <c r="J72" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K72" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J72" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K72" s="39" t="s">
+      <c r="L72" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L72" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M72" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="N72" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="N72" s="28" t="s">
+      <c r="O72" s="44" t="s">
         <v>281</v>
-      </c>
-      <c r="O72" s="44" t="s">
-        <v>282</v>
       </c>
       <c r="P72" s="29"/>
       <c r="Q72" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R72" s="66"/>
       <c r="S72" s="66"/>
@@ -6414,16 +6411,16 @@
     </row>
     <row r="73" ht="27" spans="1:28">
       <c r="A73" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B73" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B73" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C73" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E73" s="67" t="s">
         <v>21</v>
@@ -6432,35 +6429,35 @@
         <v>22</v>
       </c>
       <c r="G73" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H73" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H73" s="30" t="s">
+      <c r="I73" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I73" s="30" t="s">
+      <c r="J73" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K73" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J73" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K73" s="39" t="s">
+      <c r="L73" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L73" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M73" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N73" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O73" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P73" s="29"/>
       <c r="Q73" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R73" s="66"/>
       <c r="S73" s="66"/>
@@ -6476,16 +6473,16 @@
     </row>
     <row r="74" ht="27" spans="1:28">
       <c r="A74" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B74" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B74" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C74" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E74" s="67" t="s">
         <v>21</v>
@@ -6494,35 +6491,35 @@
         <v>22</v>
       </c>
       <c r="G74" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H74" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H74" s="30" t="s">
+      <c r="I74" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I74" s="30" t="s">
+      <c r="J74" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K74" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J74" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K74" s="39" t="s">
+      <c r="L74" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L74" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M74" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N74" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O74" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P74" s="29"/>
       <c r="Q74" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R74" s="66"/>
       <c r="S74" s="66"/>
@@ -6538,16 +6535,16 @@
     </row>
     <row r="75" ht="27" spans="1:28">
       <c r="A75" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B75" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B75" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C75" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E75" s="67" t="s">
         <v>21</v>
@@ -6556,35 +6553,35 @@
         <v>22</v>
       </c>
       <c r="G75" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H75" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H75" s="30" t="s">
+      <c r="I75" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I75" s="30" t="s">
+      <c r="J75" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K75" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J75" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K75" s="39" t="s">
+      <c r="L75" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L75" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M75" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N75" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O75" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P75" s="31"/>
       <c r="Q75" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R75" s="62"/>
       <c r="S75" s="62"/>
@@ -6600,16 +6597,16 @@
     </row>
     <row r="76" ht="27" spans="1:28">
       <c r="A76" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B76" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B76" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C76" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D76" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E76" s="67" t="s">
         <v>21</v>
@@ -6618,35 +6615,35 @@
         <v>22</v>
       </c>
       <c r="G76" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H76" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H76" s="30" t="s">
+      <c r="I76" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I76" s="30" t="s">
+      <c r="J76" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K76" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J76" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K76" s="39" t="s">
+      <c r="L76" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L76" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M76" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N76" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O76" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P76" s="31"/>
       <c r="Q76" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R76" s="62"/>
       <c r="S76" s="62"/>
@@ -6662,16 +6659,16 @@
     </row>
     <row r="77" ht="27" spans="1:28">
       <c r="A77" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B77" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B77" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C77" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D77" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E77" s="67" t="s">
         <v>21</v>
@@ -6680,35 +6677,35 @@
         <v>22</v>
       </c>
       <c r="G77" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H77" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H77" s="30" t="s">
+      <c r="I77" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I77" s="30" t="s">
+      <c r="J77" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K77" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J77" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K77" s="39" t="s">
+      <c r="L77" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L77" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M77" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N77" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O77" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P77" s="49"/>
       <c r="Q77" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R77" s="62"/>
       <c r="S77" s="62"/>
@@ -6724,16 +6721,16 @@
     </row>
     <row r="78" ht="27" spans="1:28">
       <c r="A78" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B78" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B78" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C78" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D78" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E78" s="67" t="s">
         <v>21</v>
@@ -6742,35 +6739,35 @@
         <v>22</v>
       </c>
       <c r="G78" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H78" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H78" s="30" t="s">
+      <c r="I78" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I78" s="30" t="s">
+      <c r="J78" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K78" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J78" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K78" s="39" t="s">
+      <c r="L78" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L78" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M78" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N78" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O78" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P78" s="43"/>
       <c r="Q78" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R78" s="62"/>
       <c r="S78" s="62"/>
@@ -6786,16 +6783,16 @@
     </row>
     <row r="79" ht="27" spans="1:28">
       <c r="A79" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B79" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B79" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C79" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D79" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E79" s="67" t="s">
         <v>21</v>
@@ -6804,35 +6801,35 @@
         <v>22</v>
       </c>
       <c r="G79" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H79" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H79" s="30" t="s">
+      <c r="I79" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I79" s="30" t="s">
+      <c r="J79" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K79" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J79" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K79" s="39" t="s">
+      <c r="L79" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L79" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M79" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N79" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O79" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P79" s="43"/>
       <c r="Q79" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R79" s="62"/>
       <c r="S79" s="62"/>
@@ -6848,16 +6845,16 @@
     </row>
     <row r="80" ht="27" spans="1:28">
       <c r="A80" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B80" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B80" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C80" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D80" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E80" s="67" t="s">
         <v>21</v>
@@ -6866,35 +6863,35 @@
         <v>22</v>
       </c>
       <c r="G80" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H80" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H80" s="30" t="s">
+      <c r="I80" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I80" s="30" t="s">
+      <c r="J80" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K80" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J80" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K80" s="39" t="s">
+      <c r="L80" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L80" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M80" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N80" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O80" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P80" s="47"/>
       <c r="Q80" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R80" s="62"/>
       <c r="S80" s="62"/>
@@ -6910,16 +6907,16 @@
     </row>
     <row r="81" ht="27" spans="1:28">
       <c r="A81" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B81" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B81" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="C81" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D81" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E81" s="67" t="s">
         <v>21</v>
@@ -6928,35 +6925,35 @@
         <v>22</v>
       </c>
       <c r="G81" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H81" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="H81" s="30" t="s">
+      <c r="I81" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="I81" s="30" t="s">
+      <c r="J81" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="K81" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="J81" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="K81" s="39" t="s">
+      <c r="L81" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="L81" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="M81" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N81" s="28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O81" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P81" s="48"/>
       <c r="Q81" s="65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R81" s="62"/>
       <c r="S81" s="62"/>
@@ -7012,27 +7009,27 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add iluvatar gpu card
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler22.03-LTS上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler22.03-LTS上两类平台板卡兼容清单.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20387"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwx1124290\Desktop\PR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Station\Gitee\website-v2\data\compatibility\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC31D18-5339-4437-9A3B-623374517517}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28125" windowHeight="12540" tabRatio="503"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28130" windowHeight="12540" tabRatio="503" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openEuler22.03-LTS两类平台板卡兼容性" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="328">
   <si>
     <t>vendorID</t>
   </si>
@@ -1092,12 +1093,68 @@
     </r>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
+  <si>
+    <t>1e3e</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>x86_64</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>openEuler 22.03 LTS</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>bi_driver</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>1cd1fe6796b4df2ca062aac9496e3f5b201032d26f788c0cdfe202156a0ddf5e</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>iluvatar</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>天垓加速卡(BI-V100)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>天垓芯片(BI-V100)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>商用驱动</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPU</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.06.21</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.7M</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1164,6 +1221,12 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1450,8 +1513,8 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="2"/>
-    <cellStyle name="常规 3" xfId="3"/>
+    <cellStyle name="常规 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="常规 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1792,32 +1855,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O103" sqref="O103"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.25" customWidth="1"/>
-    <col min="5" max="5" width="10.375" customWidth="1"/>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="17.875" customWidth="1"/>
-    <col min="10" max="10" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" customWidth="1"/>
+    <col min="8" max="8" width="17.90625" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" customWidth="1"/>
     <col min="11" max="11" width="41" customWidth="1"/>
-    <col min="12" max="12" width="9.625" customWidth="1"/>
-    <col min="13" max="13" width="14.75" customWidth="1"/>
-    <col min="14" max="14" width="31.125" customWidth="1"/>
-    <col min="15" max="15" width="28.125" customWidth="1"/>
-    <col min="16" max="16" width="9.375" customWidth="1"/>
+    <col min="12" max="12" width="9.6328125" customWidth="1"/>
+    <col min="13" max="13" width="14.7265625" customWidth="1"/>
+    <col min="14" max="14" width="31.08984375" customWidth="1"/>
+    <col min="15" max="15" width="28.08984375" customWidth="1"/>
+    <col min="16" max="16" width="9.36328125" customWidth="1"/>
     <col min="17" max="17" width="138" customWidth="1"/>
-    <col min="18" max="18" width="18.75" customWidth="1"/>
+    <col min="18" max="18" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1876,7 +1939,7 @@
       <c r="T1" s="30"/>
       <c r="U1" s="30"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -1933,7 +1996,7 @@
       <c r="T2" s="45"/>
       <c r="U2" s="45"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>18</v>
       </c>
@@ -1990,7 +2053,7 @@
       <c r="T3" s="45"/>
       <c r="U3" s="45"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
@@ -2047,7 +2110,7 @@
       <c r="T4" s="45"/>
       <c r="U4" s="46"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>45</v>
       </c>
@@ -2104,7 +2167,7 @@
       <c r="T5" s="45"/>
       <c r="U5" s="6"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>57</v>
       </c>
@@ -2159,7 +2222,7 @@
       <c r="T6" s="45"/>
       <c r="U6" s="6"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>45</v>
       </c>
@@ -2216,7 +2279,7 @@
       <c r="T7" s="45"/>
       <c r="U7" s="47"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>75</v>
       </c>
@@ -2269,7 +2332,7 @@
       <c r="T8" s="45"/>
       <c r="U8" s="46"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
@@ -2324,7 +2387,7 @@
       <c r="T9" s="45"/>
       <c r="U9" s="6"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>75</v>
       </c>
@@ -2379,7 +2442,7 @@
       <c r="T10" s="45"/>
       <c r="U10" s="47"/>
     </row>
-    <row r="11" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>94</v>
       </c>
@@ -2434,7 +2497,7 @@
       <c r="R11" s="12"/>
       <c r="U11" s="48"/>
     </row>
-    <row r="12" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>107</v>
       </c>
@@ -2488,7 +2551,7 @@
       </c>
       <c r="R12" s="12"/>
     </row>
-    <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>107</v>
       </c>
@@ -2541,7 +2604,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>94</v>
       </c>
@@ -2595,7 +2658,7 @@
       </c>
       <c r="U14" s="49"/>
     </row>
-    <row r="15" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>94</v>
       </c>
@@ -2649,7 +2712,7 @@
       </c>
       <c r="U15" s="48"/>
     </row>
-    <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>107</v>
       </c>
@@ -2702,7 +2765,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>107</v>
       </c>
@@ -2755,7 +2818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>94</v>
       </c>
@@ -2809,7 +2872,7 @@
       </c>
       <c r="U18" s="49"/>
     </row>
-    <row r="19" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>94</v>
       </c>
@@ -2862,7 +2925,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>94</v>
       </c>
@@ -2915,7 +2978,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>107</v>
       </c>
@@ -2969,7 +3032,7 @@
       </c>
       <c r="U21" s="48"/>
     </row>
-    <row r="22" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>57</v>
       </c>
@@ -3019,7 +3082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>57</v>
       </c>
@@ -3069,7 +3132,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>35</v>
       </c>
@@ -3123,7 +3186,7 @@
       </c>
       <c r="U24" s="49"/>
     </row>
-    <row r="25" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>18</v>
       </c>
@@ -3176,7 +3239,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>18</v>
       </c>
@@ -3229,7 +3292,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>18</v>
       </c>
@@ -3282,7 +3345,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -3335,7 +3398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>18</v>
       </c>
@@ -3388,7 +3451,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
@@ -3445,7 +3508,7 @@
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>94</v>
       </c>
@@ -3502,7 +3565,7 @@
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>45</v>
       </c>
@@ -3559,7 +3622,7 @@
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>75</v>
       </c>
@@ -3614,7 +3677,7 @@
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
     </row>
-    <row r="34" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -3668,7 +3731,7 @@
       </c>
       <c r="V34" s="60"/>
     </row>
-    <row r="35" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>107</v>
       </c>
@@ -3722,7 +3785,7 @@
       </c>
       <c r="V35" s="60"/>
     </row>
-    <row r="36" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>107</v>
       </c>
@@ -3776,7 +3839,7 @@
       </c>
       <c r="V36" s="60"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="24">
         <v>8086</v>
       </c>
@@ -3833,7 +3896,7 @@
       <c r="T37" s="5"/>
       <c r="U37" s="5"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="24">
         <v>8086</v>
       </c>
@@ -3890,7 +3953,7 @@
       <c r="T38" s="5"/>
       <c r="U38" s="5"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>75</v>
       </c>
@@ -3945,7 +4008,7 @@
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>75</v>
       </c>
@@ -4000,7 +4063,7 @@
       <c r="T40" s="5"/>
       <c r="U40" s="5"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>45</v>
       </c>
@@ -4057,7 +4120,7 @@
       <c r="T41" s="5"/>
       <c r="U41" s="5"/>
     </row>
-    <row r="42" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>45</v>
       </c>
@@ -4112,7 +4175,7 @@
       <c r="T42" s="50"/>
       <c r="U42" s="50"/>
     </row>
-    <row r="43" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>195</v>
       </c>
@@ -4167,7 +4230,7 @@
       <c r="T43" s="50"/>
       <c r="U43" s="50"/>
     </row>
-    <row r="44" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
         <v>107</v>
       </c>
@@ -4224,7 +4287,7 @@
       <c r="T44" s="50"/>
       <c r="U44" s="50"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>195</v>
       </c>
@@ -4279,7 +4342,7 @@
       <c r="T45" s="5"/>
       <c r="U45" s="5"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="27" t="s">
         <v>195</v>
       </c>
@@ -4334,7 +4397,7 @@
       <c r="T46" s="49"/>
       <c r="U46" s="5"/>
     </row>
-    <row r="47" spans="1:22" ht="27" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:22" ht="28" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>220</v>
       </c>
@@ -4389,7 +4452,7 @@
       <c r="T47" s="50"/>
       <c r="U47" s="50"/>
     </row>
-    <row r="48" spans="1:22" ht="27" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:22" ht="28" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>220</v>
       </c>
@@ -4444,7 +4507,7 @@
       <c r="T48" s="50"/>
       <c r="U48" s="50"/>
     </row>
-    <row r="49" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>234</v>
       </c>
@@ -4499,7 +4562,7 @@
       <c r="T49" s="50"/>
       <c r="U49" s="50"/>
     </row>
-    <row r="50" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>234</v>
       </c>
@@ -4554,7 +4617,7 @@
       <c r="T50" s="50"/>
       <c r="U50" s="50"/>
     </row>
-    <row r="51" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
         <v>240</v>
       </c>
@@ -4609,7 +4672,7 @@
       <c r="T51" s="50"/>
       <c r="U51" s="50"/>
     </row>
-    <row r="52" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
         <v>240</v>
       </c>
@@ -4664,7 +4727,7 @@
       <c r="T52" s="50"/>
       <c r="U52" s="50"/>
     </row>
-    <row r="53" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
         <v>240</v>
       </c>
@@ -4719,7 +4782,7 @@
       <c r="T53" s="50"/>
       <c r="U53" s="50"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
         <v>250</v>
       </c>
@@ -4764,7 +4827,7 @@
       <c r="T54" s="50"/>
       <c r="U54" s="50"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
         <v>250</v>
       </c>
@@ -4809,7 +4872,7 @@
       <c r="T55" s="50"/>
       <c r="U55" s="50"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
         <v>250</v>
       </c>
@@ -4854,7 +4917,7 @@
       <c r="T56" s="50"/>
       <c r="U56" s="50"/>
     </row>
-    <row r="57" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A57" s="30" t="s">
         <v>240</v>
       </c>
@@ -4909,7 +4972,7 @@
       <c r="T57" s="50"/>
       <c r="U57" s="50"/>
     </row>
-    <row r="58" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A58" s="30" t="s">
         <v>240</v>
       </c>
@@ -4964,7 +5027,7 @@
       <c r="T58" s="54"/>
       <c r="U58" s="54"/>
     </row>
-    <row r="59" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A59" s="30" t="s">
         <v>240</v>
       </c>
@@ -5019,7 +5082,7 @@
       <c r="T59" s="54"/>
       <c r="U59" s="54"/>
     </row>
-    <row r="60" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
         <v>240</v>
       </c>
@@ -5074,7 +5137,7 @@
       <c r="T60" s="54"/>
       <c r="U60" s="54"/>
     </row>
-    <row r="61" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
         <v>240</v>
       </c>
@@ -5129,7 +5192,7 @@
       <c r="T61" s="50"/>
       <c r="U61" s="50"/>
     </row>
-    <row r="62" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>240</v>
       </c>
@@ -5184,7 +5247,7 @@
       <c r="T62" s="50"/>
       <c r="U62" s="50"/>
     </row>
-    <row r="63" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
         <v>240</v>
       </c>
@@ -5239,7 +5302,7 @@
       <c r="T63" s="50"/>
       <c r="U63" s="50"/>
     </row>
-    <row r="64" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
         <v>240</v>
       </c>
@@ -5294,7 +5357,7 @@
       <c r="T64" s="50"/>
       <c r="U64" s="50"/>
     </row>
-    <row r="65" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
         <v>240</v>
       </c>
@@ -5349,7 +5412,7 @@
       <c r="T65" s="50"/>
       <c r="U65" s="50"/>
     </row>
-    <row r="66" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
         <v>240</v>
       </c>
@@ -5404,7 +5467,7 @@
       <c r="T66" s="50"/>
       <c r="U66" s="50"/>
     </row>
-    <row r="67" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
         <v>240</v>
       </c>
@@ -5459,7 +5522,7 @@
       <c r="T67" s="50"/>
       <c r="U67" s="50"/>
     </row>
-    <row r="68" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
         <v>240</v>
       </c>
@@ -5514,7 +5577,7 @@
       <c r="T68" s="50"/>
       <c r="U68" s="50"/>
     </row>
-    <row r="69" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>240</v>
       </c>
@@ -5569,7 +5632,7 @@
       <c r="T69" s="50"/>
       <c r="U69" s="50"/>
     </row>
-    <row r="70" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
         <v>240</v>
       </c>
@@ -5624,7 +5687,7 @@
       <c r="T70" s="50"/>
       <c r="U70" s="50"/>
     </row>
-    <row r="71" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
         <v>240</v>
       </c>
@@ -5679,7 +5742,7 @@
       <c r="T71" s="50"/>
       <c r="U71" s="50"/>
     </row>
-    <row r="72" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>240</v>
       </c>
@@ -5734,7 +5797,7 @@
       <c r="T72" s="54"/>
       <c r="U72" s="54"/>
     </row>
-    <row r="73" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
         <v>240</v>
       </c>
@@ -5789,7 +5852,7 @@
       <c r="T73" s="54"/>
       <c r="U73" s="54"/>
     </row>
-    <row r="74" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
         <v>240</v>
       </c>
@@ -5844,7 +5907,7 @@
       <c r="T74" s="54"/>
       <c r="U74" s="54"/>
     </row>
-    <row r="75" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
         <v>240</v>
       </c>
@@ -5899,7 +5962,7 @@
       <c r="T75" s="50"/>
       <c r="U75" s="50"/>
     </row>
-    <row r="76" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
         <v>240</v>
       </c>
@@ -5954,7 +6017,7 @@
       <c r="T76" s="50"/>
       <c r="U76" s="50"/>
     </row>
-    <row r="77" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
         <v>240</v>
       </c>
@@ -6009,7 +6072,7 @@
       <c r="T77" s="50"/>
       <c r="U77" s="50"/>
     </row>
-    <row r="78" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
         <v>240</v>
       </c>
@@ -6064,7 +6127,7 @@
       <c r="T78" s="50"/>
       <c r="U78" s="50"/>
     </row>
-    <row r="79" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
         <v>240</v>
       </c>
@@ -6119,7 +6182,7 @@
       <c r="T79" s="50"/>
       <c r="U79" s="50"/>
     </row>
-    <row r="80" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
         <v>240</v>
       </c>
@@ -6174,7 +6237,7 @@
       <c r="T80" s="50"/>
       <c r="U80" s="50"/>
     </row>
-    <row r="81" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:21" ht="28" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
         <v>240</v>
       </c>
@@ -6229,7 +6292,7 @@
       <c r="T81" s="50"/>
       <c r="U81" s="50"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>18</v>
       </c>
@@ -6286,7 +6349,7 @@
       <c r="T82" s="45"/>
       <c r="U82" s="45"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>18</v>
       </c>
@@ -6343,7 +6406,7 @@
       <c r="T83" s="45"/>
       <c r="U83" s="45"/>
     </row>
-    <row r="84" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="50" t="s">
         <v>35</v>
       </c>
@@ -6388,7 +6451,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="50" t="s">
         <v>35</v>
       </c>
@@ -6433,7 +6496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="50" t="s">
         <v>35</v>
       </c>
@@ -6478,7 +6541,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="50" t="s">
         <v>35</v>
       </c>
@@ -6523,21 +6586,66 @@
         <v>32</v>
       </c>
     </row>
+    <row r="88" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="50" t="s">
+        <v>314</v>
+      </c>
+      <c r="B88" s="56" t="s">
+        <v>315</v>
+      </c>
+      <c r="E88" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="F88" s="57" t="s">
+        <v>317</v>
+      </c>
+      <c r="G88" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="H88" s="57" t="s">
+        <v>325</v>
+      </c>
+      <c r="I88" s="50" t="s">
+        <v>324</v>
+      </c>
+      <c r="J88" s="50" t="s">
+        <v>326</v>
+      </c>
+      <c r="K88" s="50" t="s">
+        <v>319</v>
+      </c>
+      <c r="L88" s="57" t="s">
+        <v>327</v>
+      </c>
+      <c r="M88" s="50" t="s">
+        <v>320</v>
+      </c>
+      <c r="N88" s="50" t="s">
+        <v>321</v>
+      </c>
+      <c r="O88" s="50" t="s">
+        <v>322</v>
+      </c>
+      <c r="P88" s="56"/>
+      <c r="Q88" s="50" t="s">
+        <v>323</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:U87"/>
+  <autoFilter ref="A1:U87" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10 E47:E67 E82:E83">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10 E47:E67 E82:E83" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"aarch64,x86_64"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="Q10" r:id="rId1"/>
-    <hyperlink ref="Q8" r:id="rId2"/>
-    <hyperlink ref="Q33" r:id="rId3"/>
-    <hyperlink ref="Q39" r:id="rId4"/>
-    <hyperlink ref="Q40" r:id="rId5"/>
-    <hyperlink ref="Q47" r:id="rId6"/>
+    <hyperlink ref="Q10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="Q8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="Q33" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="Q39" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="Q40" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="Q47" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
@@ -6545,22 +6653,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="1" customWidth="1"/>
     <col min="4" max="1024" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>271</v>
       </c>
@@ -6569,7 +6677,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>181</v>
       </c>
@@ -6577,7 +6685,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>181</v>
       </c>

</xml_diff>